<commit_message>
feat: patch release 3.0.1
Patch release 3.0.1:

- Expanded on [filtering logic](#filtering)
- Clarified description of [filtering parameters](#parameters).
- Added extra examples.
- Removed invalid geography properties in some examples.
- Expanded on `declaredUnitofMeasurement` description.
- Added removal of `biogenicAccountingMethodology` to changelog of [3.0.0](#changelog-3.0.0)
</commit_message>
<xml_diff>
--- a/data-exchange-protocol/latest/pact-simplified.xlsx
+++ b/data-exchange-protocol/latest/pact-simplified.xlsx
@@ -569,7 +569,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>3.0.0</t>
+          <t>3.0.1</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
@@ -1606,7 +1606,7 @@
       <c r="E21" s="12" t="inlineStr">
         <is>
           <t>The unit of measurement of the product. Together with `declaredUnitAmount` this defines the 'declared unit' of the product. Emissions in this carbon footprint are expressed in kgCO2e per 'declared unit'. 
-For example: a PCF for a 12 liter bottle of Ethanol states 2 kg of CO2e in emissions. In this case the declared unit is 12 liter Ethanol, thus the `declaredUnitOfMeasurement` is "liter", and the `declaredUnitAmount` is 12.</t>
+For example: a PCF for a 12.5 liter bottle of Ethanol states 2 kg of CO2e in emissions. In this case the declared unit is 12.5 liter Ethanol, thus the `declaredUnitOfMeasurement` is "liter", and the `declaredUnitAmount` is "12.5". The `pcfIncludingBiogenicUptake` is "2.0" kgCO2e per "12.5 liter" of Ethanol.</t>
         </is>
       </c>
       <c r="F21" s="11" t="inlineStr">
@@ -1953,21 +1953,9 @@
 (string)</t>
         </is>
       </c>
-      <c r="J26" s="12" t="inlineStr">
-        <is>
-          <t>Northern America</t>
-        </is>
-      </c>
-      <c r="K26" s="12" t="inlineStr">
-        <is>
-          <t>Northern America</t>
-        </is>
-      </c>
-      <c r="L26" s="12" t="inlineStr">
-        <is>
-          <t>Northern Europe</t>
-        </is>
-      </c>
+      <c r="J26" s="12" t="inlineStr"/>
+      <c r="K26" s="12" t="inlineStr"/>
+      <c r="L26" s="12" t="inlineStr"/>
       <c r="M26" s="12" t="inlineStr">
         <is>
           <t>Latin America and the Caribbean</t>
@@ -2017,26 +2005,14 @@
 (string)</t>
         </is>
       </c>
-      <c r="J27" s="12" t="inlineStr">
+      <c r="J27" s="12" t="inlineStr"/>
+      <c r="K27" s="12" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="K27" s="12" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="L27" s="12" t="inlineStr">
-        <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="M27" s="12" t="inlineStr">
-        <is>
-          <t>BR</t>
-        </is>
-      </c>
+      <c r="L27" s="12" t="inlineStr"/>
+      <c r="M27" s="12" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="9" t="inlineStr">
@@ -2086,21 +2062,13 @@
           <t>US-TX</t>
         </is>
       </c>
-      <c r="K28" s="12" t="inlineStr">
-        <is>
-          <t>US-TX</t>
-        </is>
-      </c>
+      <c r="K28" s="12" t="inlineStr"/>
       <c r="L28" s="12" t="inlineStr">
         <is>
           <t>DE-BW</t>
         </is>
       </c>
-      <c r="M28" s="12" t="inlineStr">
-        <is>
-          <t>BR-SP</t>
-        </is>
-      </c>
+      <c r="M28" s="12" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="9" t="inlineStr">
@@ -3850,7 +3818,7 @@
       </c>
       <c r="I57" s="12" t="inlineStr">
         <is>
-          <t>array: ISO14067|ISO14083|ISO14040-44|GHGP-Product|PEF|PACT-1.0|PACT-2.0|PACT-3.0
+          <t>array: ISO14067|ISO14083|ISO14040-44|GHGP-Product|PEF|PACT-1.0|PACT-2.0|PACT-3.0|PAS2050|...
 (string)</t>
         </is>
       </c>
@@ -3871,7 +3839,7 @@
       </c>
       <c r="M57" s="12" t="inlineStr">
         <is>
-          <t>['PEF']</t>
+          <t>['PEF', 'FUTURE-STANDARD']</t>
         </is>
       </c>
     </row>

</xml_diff>